<commit_message>
Made some changes, that's it
</commit_message>
<xml_diff>
--- a/OrderData/completed.xlsx
+++ b/OrderData/completed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{52C301B5-F66D-4C76-84D4-CF139CFD6B34}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D2C1518D-FBD4-4E15-AB3B-09632FEDEDC4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>SN</t>
   </si>
@@ -115,19 +115,13 @@
     <t>Completed Date</t>
   </si>
   <si>
-    <t>Exit Price</t>
-  </si>
-  <si>
-    <t>Exit Price1</t>
-  </si>
-  <si>
-    <t>Exit Price2</t>
-  </si>
-  <si>
-    <t>Exit Price3</t>
-  </si>
-  <si>
-    <t>Exit Price4</t>
+    <t>CurrentSop</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Product</t>
   </si>
 </sst>
 </file>
@@ -446,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,14 +469,14 @@
     <col min="27" max="27" width="10.77734375" customWidth="1"/>
     <col min="28" max="28" width="11.109375" customWidth="1"/>
     <col min="31" max="31" width="15.6640625" customWidth="1"/>
-    <col min="32" max="32" width="10.33203125" customWidth="1"/>
-    <col min="33" max="33" width="10.5546875" customWidth="1"/>
+    <col min="32" max="32" width="12.5546875" customWidth="1"/>
+    <col min="33" max="33" width="14.6640625" customWidth="1"/>
     <col min="34" max="34" width="10.44140625" customWidth="1"/>
     <col min="35" max="35" width="11.109375" customWidth="1"/>
     <col min="36" max="36" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,29 +561,23 @@
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>